<commit_message>
Version after demoted barnacles and shortly before submission - just need to add a few more dataset names
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Actinopterygii.xlsx
+++ b/data/dataPaper-I-in/arphified/Actinopterygii.xlsx
@@ -1581,76 +1581,76 @@
     <t>${catalogNumber}</t>
   </si>
   <si>
+    <t>${recordedBy}</t>
+  </si>
+  <si>
+    <t>${individualCount}</t>
+  </si>
+  <si>
+    <t>${sex}</t>
+  </si>
+  <si>
+    <t>PRESENT</t>
+  </si>
+  <si>
+    <t>${taxonName}</t>
+  </si>
+  <si>
+    <t>!references.ref</t>
+  </si>
+  <si>
+    <t>iNaturalist:${iNaturalistTaxonId}</t>
+  </si>
+  <si>
+    <t>${scientificName}</t>
+  </si>
+  <si>
+    <t>${kingdom}</t>
+  </si>
+  <si>
+    <t>${phylum}</t>
+  </si>
+  <si>
+    <t>${class}</t>
+  </si>
+  <si>
+    <t>${order}</t>
+  </si>
+  <si>
+    <t>${family}</t>
+  </si>
+  <si>
+    <t>${genus}</t>
+  </si>
+  <si>
+    <t>${subgenus}</t>
+  </si>
+  <si>
+    <t>Galiano Island</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>British Columbia</t>
+  </si>
+  <si>
+    <t>${locality}</t>
+  </si>
+  <si>
+    <t>${depth}</t>
+  </si>
+  <si>
+    <t>${latitude}</t>
+  </si>
+  <si>
+    <t>${longitude}</t>
+  </si>
+  <si>
     <t>Confidence: ${confidence}</t>
-  </si>
-  <si>
-    <t>${recordedBy}</t>
-  </si>
-  <si>
-    <t>${individualCount}</t>
-  </si>
-  <si>
-    <t>${sex}</t>
-  </si>
-  <si>
-    <t>PRESENT</t>
-  </si>
-  <si>
-    <t>${taxonName}</t>
-  </si>
-  <si>
-    <t>!references.ref</t>
-  </si>
-  <si>
-    <t>iNaturalist:${iNaturalistTaxonId}</t>
-  </si>
-  <si>
-    <t>${scientificName}</t>
-  </si>
-  <si>
-    <t>${kingdom}</t>
-  </si>
-  <si>
-    <t>${phylum}</t>
-  </si>
-  <si>
-    <t>${class}</t>
-  </si>
-  <si>
-    <t>${order}</t>
-  </si>
-  <si>
-    <t>${family}</t>
-  </si>
-  <si>
-    <t>${genus}</t>
-  </si>
-  <si>
-    <t>${subgenus}</t>
-  </si>
-  <si>
-    <t>Galiano Island</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>British Columbia</t>
-  </si>
-  <si>
-    <t>${locality}</t>
-  </si>
-  <si>
-    <t>${depth}</t>
-  </si>
-  <si>
-    <t>${latitude}</t>
-  </si>
-  <si>
-    <t>${longitude}</t>
   </si>
   <si>
     <t>!references.samplingProtocol</t>
@@ -10789,301 +10789,301 @@
         <v>36</v>
       </c>
       <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
         <v>522</v>
       </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
         <v>523</v>
       </c>
-      <c r="I2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>524</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
         <v>525</v>
       </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
         <v>526</v>
       </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
         <v>527</v>
       </c>
-      <c r="U2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
         <v>528</v>
       </c>
-      <c r="W2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG2" t="s">
         <v>529</v>
       </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN2" t="s">
         <v>530</v>
       </c>
-      <c r="AH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>531</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>532</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>533</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>534</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>535</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>536</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BK2" t="s">
         <v>537</v>
       </c>
-      <c r="AU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BK2" t="s">
+      <c r="BL2" t="s">
         <v>538</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
         <v>539</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BN2" t="s">
         <v>540</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BQ2" t="s">
         <v>541</v>
       </c>
-      <c r="BO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BQ2" t="s">
+      <c r="BR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV2" t="s">
         <v>542</v>
       </c>
-      <c r="BR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BV2" t="s">
+      <c r="BW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CH2" t="s">
         <v>543</v>
       </c>
-      <c r="BW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CH2" t="s">
+      <c r="CI2" t="s">
         <v>544</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="CJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>522</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ2" t="s">
         <v>545</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>523</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>36</v>
       </c>
       <c r="DA2" t="s">
         <v>36</v>
@@ -11206,7 +11206,7 @@
         <v>36</v>
       </c>
       <c r="EO2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="EP2" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Partway through addressing technical review - coordinates rounded, and propagated some coordinate uncertainties
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Actinopterygii.xlsx
+++ b/data/dataPaper-I-in/arphified/Actinopterygii.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="561">
   <si>
     <t>Taxon_Local_ID</t>
   </si>
@@ -1648,6 +1648,9 @@
   </si>
   <si>
     <t>${longitude}</t>
+  </si>
+  <si>
+    <t>${coordinateUncertaintyInMeters}</t>
   </si>
   <si>
     <t>Confidence: ${confidence}</t>
@@ -11038,7 +11041,7 @@
         <v>36</v>
       </c>
       <c r="CK2" t="s">
-        <v>36</v>
+        <v>545</v>
       </c>
       <c r="CL2" t="s">
         <v>36</v>
@@ -11083,7 +11086,7 @@
         <v>36</v>
       </c>
       <c r="CZ2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="DA2" t="s">
         <v>36</v>
@@ -11146,13 +11149,13 @@
         <v>36</v>
       </c>
       <c r="DU2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="DV2" t="s">
         <v>36</v>
       </c>
       <c r="DW2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="DX2" t="s">
         <v>36</v>
@@ -11164,13 +11167,13 @@
         <v>36</v>
       </c>
       <c r="EA2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="EB2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="EC2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="ED2" t="s">
         <v>36</v>
@@ -11179,13 +11182,13 @@
         <v>36</v>
       </c>
       <c r="EF2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="EG2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="EH2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="EI2" t="s">
         <v>36</v>
@@ -11218,19 +11221,19 @@
         <v>36</v>
       </c>
       <c r="ES2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="ET2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="EU2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="EV2" t="s">
         <v>36</v>
       </c>
       <c r="EW2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="EX2" t="s">
         <v>36</v>
@@ -11261,10 +11264,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First version in which all technical review comments are notionally addressed
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Actinopterygii.xlsx
+++ b/data/dataPaper-I-in/arphified/Actinopterygii.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="569">
   <si>
     <t>Taxon_Local_ID</t>
   </si>
@@ -249,7 +249,7 @@
     <t>Linnaeus, 1758</t>
   </si>
   <si>
-    <t>"Due to the species’ tendency for genetic variability among isolated populations, Jack Creek’s three spine sticklebacks may be a rare sub-species. This investigation was never followed up" (Keith Erickson, pers. comm 2020).</t>
+    <t>"Due to the genetic variability exhibited among isolated populations, Jack Creek’s three spine sticklebacks may be a rare sub-species. This investigation was never followed up" (Keith Erickson pers. comm 2020).</t>
   </si>
   <si>
     <t>67409</t>
@@ -1230,6 +1230,15 @@
     <t>order</t>
   </si>
   <si>
+    <t>suborder</t>
+  </si>
+  <si>
+    <t>infraorder</t>
+  </si>
+  <si>
+    <t>superfamily</t>
+  </si>
+  <si>
     <t>family</t>
   </si>
   <si>
@@ -1602,7 +1611,7 @@
     <t>iNaturalist:${iNaturalistTaxonId}</t>
   </si>
   <si>
-    <t>${scientificName}</t>
+    <t>${summary.taxonName}</t>
   </si>
   <si>
     <t>${kingdom}</t>
@@ -1617,6 +1626,15 @@
     <t>${order}</t>
   </si>
   <si>
+    <t>${suborder}</t>
+  </si>
+  <si>
+    <t>${infraorder}</t>
+  </si>
+  <si>
+    <t>${superfamily}</t>
+  </si>
+  <si>
     <t>${family}</t>
   </si>
   <si>
@@ -1626,6 +1644,9 @@
     <t>${subgenus}</t>
   </si>
   <si>
+    <t>${summary.Author}</t>
+  </si>
+  <si>
     <t>Galiano Island</t>
   </si>
   <si>
@@ -1660,6 +1681,9 @@
   </si>
   <si>
     <t>!Date:YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>!Date:HH:mm:ss</t>
   </si>
   <si>
     <t>!Date:YYYY</t>
@@ -10299,10 +10323,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FA2"/>
+  <dimension ref="A1:FD2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10774,19 +10798,28 @@
       <c r="FA1" t="s">
         <v>518</v>
       </c>
+      <c r="FB1" t="s">
+        <v>519</v>
+      </c>
+      <c r="FC1" t="s">
+        <v>520</v>
+      </c>
+      <c r="FD1" t="s">
+        <v>521</v>
+      </c>
     </row>
-    <row r="2" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="D2" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
@@ -10798,16 +10831,16 @@
         <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="I2" t="s">
         <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="K2" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="L2" t="s">
         <v>36</v>
@@ -10822,429 +10855,438 @@
         <v>36</v>
       </c>
       <c r="P2" t="s">
+        <v>528</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>529</v>
+      </c>
+      <c r="U2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
+        <v>530</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>531</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>532</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>535</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>536</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>537</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>538</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>539</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>540</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>541</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>542</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>543</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>544</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>545</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>546</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>547</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>548</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>549</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>550</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>551</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>552</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT2" t="s">
         <v>525</v>
       </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>526</v>
-      </c>
-      <c r="U2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" t="s">
-        <v>527</v>
-      </c>
-      <c r="W2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>528</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>529</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN2" t="s">
+      <c r="CU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>553</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>554</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>555</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>556</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>557</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>558</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>559</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>560</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>561</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>562</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ER2" t="s">
         <v>530</v>
       </c>
-      <c r="AO2" t="s">
-        <v>531</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>532</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>533</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>534</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>535</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>536</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>537</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>538</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>539</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>540</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>541</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>542</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>543</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>544</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>545</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>522</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>546</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>547</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>548</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>549</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>550</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>551</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>552</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>553</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>554</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>527</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>36</v>
-      </c>
       <c r="ES2" t="s">
-        <v>555</v>
+        <v>36</v>
       </c>
       <c r="ET2" t="s">
-        <v>556</v>
+        <v>36</v>
       </c>
       <c r="EU2" t="s">
-        <v>557</v>
+        <v>36</v>
       </c>
       <c r="EV2" t="s">
-        <v>36</v>
+        <v>563</v>
       </c>
       <c r="EW2" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="EX2" t="s">
-        <v>36</v>
+        <v>565</v>
       </c>
       <c r="EY2" t="s">
         <v>36</v>
       </c>
       <c r="EZ2" t="s">
-        <v>36</v>
+        <v>566</v>
       </c>
       <c r="FA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="FB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="FD2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -11264,10 +11306,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>559</v>
+        <v>567</v>
       </c>
       <c r="C1" t="s">
-        <v>560</v>
+        <v>568</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed up Myxicola and a few more loose ends in second review
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Actinopterygii.xlsx
+++ b/data/dataPaper-I-in/arphified/Actinopterygii.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="562">
   <si>
     <t>Taxon_Local_ID</t>
   </si>
@@ -1230,15 +1230,6 @@
     <t>order</t>
   </si>
   <si>
-    <t>suborder</t>
-  </si>
-  <si>
-    <t>infraorder</t>
-  </si>
-  <si>
-    <t>superfamily</t>
-  </si>
-  <si>
     <t>family</t>
   </si>
   <si>
@@ -1581,9 +1572,6 @@
     <t>source</t>
   </si>
   <si>
-    <t>${iNaturalistTaxonId}</t>
-  </si>
-  <si>
     <t>${gbifOccurrenceID}</t>
   </si>
   <si>
@@ -1626,15 +1614,6 @@
     <t>${order}</t>
   </si>
   <si>
-    <t>${suborder}</t>
-  </si>
-  <si>
-    <t>${infraorder}</t>
-  </si>
-  <si>
-    <t>${superfamily}</t>
-  </si>
-  <si>
     <t>${family}</t>
   </si>
   <si>
@@ -1644,7 +1623,7 @@
     <t>${subgenus}</t>
   </si>
   <si>
-    <t>${summary.Author}</t>
+    <t>${summary.authority}</t>
   </si>
   <si>
     <t>Galiano Island</t>
@@ -10323,970 +10302,946 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FD2"/>
+  <dimension ref="A1:EZ2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="G1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="H1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="I1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="J1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="K1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="L1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="M1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="N1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="O1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="P1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="Q1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="R1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="S1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="T1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="U1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="V1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="W1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="X1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="Y1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="Z1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AA1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AB1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AC1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AD1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AE1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AF1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AG1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AH1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AI1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AJ1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AK1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AL1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AM1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AN1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AO1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AP1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AQ1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AR1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AS1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AT1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AU1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AV1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AW1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AX1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AY1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AZ1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="BA1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="BB1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="BC1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="BD1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="BE1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="BF1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="BG1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="BH1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="BI1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="BJ1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="BK1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="BL1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="BM1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="BN1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="BO1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="BP1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="BQ1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="BR1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="BS1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="BT1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="BU1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="BV1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="BW1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="BX1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="BY1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="BZ1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="CA1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CB1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="CC1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="CD1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="CE1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="CF1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="CG1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="CH1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="CI1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="CJ1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="CK1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="CL1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="CM1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="CN1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="CO1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="CP1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="CQ1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="CR1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="CS1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="CT1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="CU1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="CV1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="CW1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="CX1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="CY1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="CZ1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="DA1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="DB1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="DC1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="DD1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="DE1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="DF1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="DG1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="DH1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="DI1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="DJ1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="DK1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="DL1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="DM1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="DN1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="DO1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="DP1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="DQ1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="DR1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="DS1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="DT1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="DU1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="DV1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="DW1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="DX1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="DY1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="DZ1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="EA1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="EB1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="EC1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="ED1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="EE1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="EF1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="EG1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="EH1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="EI1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="EJ1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="EK1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="EL1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="EM1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="EN1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="EO1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="EP1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="EQ1" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="ER1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="ES1" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="ET1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="EU1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="EV1" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="EW1" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="EX1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="EY1" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="EZ1" t="s">
-        <v>517</v>
-      </c>
-      <c r="FA1" t="s">
         <v>518</v>
       </c>
-      <c r="FB1" t="s">
+    </row>
+    <row r="2" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>519</v>
       </c>
-      <c r="FC1" t="s">
+      <c r="C2" t="s">
         <v>520</v>
       </c>
-      <c r="FD1" t="s">
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="2" spans="1:160" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
         <v>522</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="J2" t="s">
         <v>523</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
         <v>524</v>
       </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
         <v>525</v>
       </c>
-      <c r="I2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
         <v>526</v>
       </c>
-      <c r="K2" t="s">
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
         <v>527</v>
       </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Y2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
         <v>528</v>
       </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="AG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" t="s">
         <v>529</v>
       </c>
-      <c r="U2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="AN2" t="s">
         <v>530</v>
       </c>
-      <c r="W2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="AO2" t="s">
         <v>531</v>
       </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AP2" t="s">
         <v>532</v>
       </c>
-      <c r="AH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN2" t="s">
+      <c r="AQ2" t="s">
         <v>533</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AR2" t="s">
         <v>534</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AS2" t="s">
         <v>535</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX2" t="s">
         <v>536</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BJ2" t="s">
         <v>537</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="BK2" t="s">
         <v>538</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="BL2" t="s">
         <v>539</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BM2" t="s">
         <v>540</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="BN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BP2" t="s">
         <v>541</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="BQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BU2" t="s">
         <v>542</v>
       </c>
-      <c r="AX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB2" t="s">
+      <c r="BV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CG2" t="s">
         <v>543</v>
       </c>
-      <c r="BC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BN2" t="s">
+      <c r="CH2" t="s">
         <v>544</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="CI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CJ2" t="s">
         <v>545</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="CK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>521</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY2" t="s">
         <v>546</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="CZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT2" t="s">
         <v>547</v>
       </c>
-      <c r="BR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BT2" t="s">
+      <c r="DU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DV2" t="s">
         <v>548</v>
       </c>
-      <c r="BU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BY2" t="s">
+      <c r="DW2" t="s">
         <v>549</v>
       </c>
-      <c r="BZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CK2" t="s">
+      <c r="DX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DZ2" t="s">
         <v>550</v>
       </c>
-      <c r="CL2" t="s">
+      <c r="EA2" t="s">
         <v>551</v>
       </c>
-      <c r="CM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CN2" t="s">
+      <c r="EB2" t="s">
         <v>552</v>
       </c>
-      <c r="CO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>525</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DC2" t="s">
+      <c r="EC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EE2" t="s">
         <v>553</v>
       </c>
-      <c r="DD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DX2" t="s">
+      <c r="EF2" t="s">
         <v>554</v>
       </c>
-      <c r="DY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DZ2" t="s">
+      <c r="EG2" t="s">
         <v>555</v>
       </c>
-      <c r="EA2" t="s">
+      <c r="EH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>526</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ER2" t="s">
         <v>556</v>
       </c>
-      <c r="EB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ED2" t="s">
+      <c r="ES2" t="s">
         <v>557</v>
       </c>
-      <c r="EE2" t="s">
+      <c r="ET2" t="s">
         <v>558</v>
       </c>
-      <c r="EF2" t="s">
+      <c r="EU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EV2" t="s">
         <v>559</v>
       </c>
-      <c r="EG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>560</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>561</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>562</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>530</v>
-      </c>
-      <c r="ES2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ET2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EV2" t="s">
-        <v>563</v>
-      </c>
       <c r="EW2" t="s">
-        <v>564</v>
+        <v>36</v>
       </c>
       <c r="EX2" t="s">
-        <v>565</v>
+        <v>36</v>
       </c>
       <c r="EY2" t="s">
         <v>36</v>
       </c>
       <c r="EZ2" t="s">
-        <v>566</v>
-      </c>
-      <c r="FA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="FB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="FC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="FD2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -11306,10 +11261,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="C1" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrections following third round of review
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Actinopterygii.xlsx
+++ b/data/dataPaper-I-in/arphified/Actinopterygii.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3002" uniqueCount="560">
   <si>
     <t>Taxon_Local_ID</t>
   </si>
@@ -1236,9 +1236,6 @@
     <t>genus</t>
   </si>
   <si>
-    <t>subgenus</t>
-  </si>
-  <si>
     <t>specificEpithet</t>
   </si>
   <si>
@@ -1618,9 +1615,6 @@
   </si>
   <si>
     <t>${genus}</t>
-  </si>
-  <si>
-    <t>${subgenus}</t>
   </si>
   <si>
     <t>${summary.authority}</t>
@@ -10302,10 +10296,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EZ2"/>
+  <dimension ref="A1:EY2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:155" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>363</v>
       </c>
@@ -10771,466 +10765,463 @@
       <c r="EY1" t="s">
         <v>517</v>
       </c>
-      <c r="EZ1" t="s">
+    </row>
+    <row r="2" spans="1:155" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="2" spans="1:156" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>519</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
         <v>520</v>
       </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
         <v>521</v>
       </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>522</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
         <v>523</v>
       </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
         <v>524</v>
       </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
         <v>525</v>
       </c>
-      <c r="T2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
         <v>526</v>
       </c>
-      <c r="V2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
         <v>527</v>
       </c>
-      <c r="Y2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" t="s">
         <v>528</v>
       </c>
-      <c r="AG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>529</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>530</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>531</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>532</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>533</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW2" t="s">
         <v>534</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI2" t="s">
         <v>535</v>
       </c>
-      <c r="AT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX2" t="s">
+      <c r="BJ2" t="s">
         <v>536</v>
       </c>
-      <c r="AY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BJ2" t="s">
+      <c r="BK2" t="s">
         <v>537</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BL2" t="s">
         <v>538</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BO2" t="s">
         <v>539</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT2" t="s">
         <v>540</v>
       </c>
-      <c r="BN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BP2" t="s">
+      <c r="BU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF2" t="s">
         <v>541</v>
       </c>
-      <c r="BQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BU2" t="s">
+      <c r="CG2" t="s">
         <v>542</v>
       </c>
-      <c r="BV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CG2" t="s">
+      <c r="CH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI2" t="s">
         <v>543</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>520</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX2" t="s">
         <v>544</v>
       </c>
-      <c r="CI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CJ2" t="s">
+      <c r="CY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS2" t="s">
         <v>545</v>
       </c>
-      <c r="CK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>521</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CY2" t="s">
+      <c r="DT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU2" t="s">
         <v>546</v>
       </c>
-      <c r="CZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DT2" t="s">
+      <c r="DV2" t="s">
         <v>547</v>
       </c>
-      <c r="DU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DV2" t="s">
+      <c r="DW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DY2" t="s">
         <v>548</v>
       </c>
-      <c r="DW2" t="s">
+      <c r="DZ2" t="s">
         <v>549</v>
       </c>
-      <c r="DX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DZ2" t="s">
+      <c r="EA2" t="s">
         <v>550</v>
       </c>
-      <c r="EA2" t="s">
+      <c r="EB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED2" t="s">
         <v>551</v>
       </c>
-      <c r="EB2" t="s">
+      <c r="EE2" t="s">
         <v>552</v>
       </c>
-      <c r="EC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EE2" t="s">
+      <c r="EF2" t="s">
         <v>553</v>
       </c>
-      <c r="EF2" t="s">
+      <c r="EG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>525</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ2" t="s">
         <v>554</v>
       </c>
-      <c r="EG2" t="s">
+      <c r="ER2" t="s">
         <v>555</v>
       </c>
-      <c r="EH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>526</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ER2" t="s">
+      <c r="ES2" t="s">
         <v>556</v>
       </c>
-      <c r="ES2" t="s">
+      <c r="ET2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EU2" t="s">
         <v>557</v>
       </c>
-      <c r="ET2" t="s">
-        <v>558</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>36</v>
-      </c>
       <c r="EV2" t="s">
-        <v>559</v>
+        <v>36</v>
       </c>
       <c r="EW2" t="s">
         <v>36</v>
@@ -11239,9 +11230,6 @@
         <v>36</v>
       </c>
       <c r="EY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EZ2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -11261,10 +11249,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>